<commit_message>
SAV stats file fix (SBAP had duplicate records)
</commit_message>
<xml_diff>
--- a/SAV/output/website/SAV_BBpct_LMEresults_All.xlsx
+++ b/SAV/output/website/SAV_BBpct_LMEresults_All.xlsx
@@ -10005,13 +10005,13 @@
         <v>1</v>
       </c>
       <c r="M194" t="n">
-        <v>84.4240525929707</v>
+        <v>84.4240875767503</v>
       </c>
       <c r="N194" t="n">
-        <v>-2.62425693324902</v>
+        <v>-2.62425821800902</v>
       </c>
       <c r="O194" t="n">
-        <v>0.0740357901071176</v>
+        <v>0.0740365212949048</v>
       </c>
       <c r="P194" t="s">
         <v>23</v>
@@ -10025,28 +10025,28 @@
         <v>114</v>
       </c>
       <c r="C195" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D195" t="s">
         <v>18</v>
       </c>
       <c r="E195" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F195" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="G195" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="H195" t="n">
-        <v>133</v>
+        <v>460</v>
       </c>
       <c r="I195" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J195" t="n">
-        <v>2016</v>
+        <v>2000</v>
       </c>
       <c r="K195" t="n">
         <v>2023</v>
@@ -10055,13 +10055,13 @@
         <v>1</v>
       </c>
       <c r="M195" t="n">
-        <v>84.4240875767503</v>
+        <v>11.9869803993408</v>
       </c>
       <c r="N195" t="n">
-        <v>-2.62425821800902</v>
+        <v>0.27052871964274</v>
       </c>
       <c r="O195" t="n">
-        <v>0.0740365212949048</v>
+        <v>0.485492239750769</v>
       </c>
       <c r="P195" t="s">
         <v>23</v>
@@ -10075,28 +10075,28 @@
         <v>114</v>
       </c>
       <c r="C196" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D196" t="s">
         <v>18</v>
       </c>
       <c r="E196" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="G196" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="H196" t="n">
-        <v>460</v>
+        <v>76</v>
       </c>
       <c r="I196" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J196" t="n">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="K196" t="n">
         <v>2023</v>
@@ -10104,17 +10104,11 @@
       <c r="L196" t="b">
         <v>1</v>
       </c>
-      <c r="M196" t="n">
-        <v>11.9869804005955</v>
-      </c>
-      <c r="N196" t="n">
-        <v>0.270528719596189</v>
-      </c>
-      <c r="O196" t="n">
-        <v>0.485492239588718</v>
-      </c>
+      <c r="M196"/>
+      <c r="N196"/>
+      <c r="O196"/>
       <c r="P196" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="197">
@@ -10125,7 +10119,7 @@
         <v>114</v>
       </c>
       <c r="C197" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D197" t="s">
         <v>18</v>
@@ -10140,10 +10134,10 @@
         <v>116</v>
       </c>
       <c r="H197" t="n">
-        <v>460</v>
+        <v>432</v>
       </c>
       <c r="I197" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J197" t="n">
         <v>2000</v>
@@ -10155,13 +10149,13 @@
         <v>1</v>
       </c>
       <c r="M197" t="n">
-        <v>11.9869803993408</v>
+        <v>4.17288209344542</v>
       </c>
       <c r="N197" t="n">
-        <v>0.27052871964274</v>
+        <v>-0.151399197205583</v>
       </c>
       <c r="O197" t="n">
-        <v>0.485492239750769</v>
+        <v>0.819587742428702</v>
       </c>
       <c r="P197" t="s">
         <v>23</v>
@@ -10175,28 +10169,28 @@
         <v>114</v>
       </c>
       <c r="C198" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D198" t="s">
         <v>18</v>
       </c>
       <c r="E198" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F198" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="G198" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="H198" t="n">
-        <v>76</v>
+        <v>841</v>
       </c>
       <c r="I198" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J198" t="n">
-        <v>2016</v>
+        <v>2000</v>
       </c>
       <c r="K198" t="n">
         <v>2023</v>
@@ -10204,11 +10198,17 @@
       <c r="L198" t="b">
         <v>1</v>
       </c>
-      <c r="M198"/>
-      <c r="N198"/>
-      <c r="O198"/>
+      <c r="M198" t="n">
+        <v>27.0389702137899</v>
+      </c>
+      <c r="N198" t="n">
+        <v>1.06249136556588</v>
+      </c>
+      <c r="O198" t="n">
+        <v>0.131535963423934</v>
+      </c>
       <c r="P198" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="199">
@@ -10219,43 +10219,43 @@
         <v>114</v>
       </c>
       <c r="C199" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D199" t="s">
         <v>18</v>
       </c>
       <c r="E199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F199" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G199" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H199" t="n">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="I199" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J199" t="n">
         <v>2000</v>
       </c>
       <c r="K199" t="n">
-        <v>2023</v>
+        <v>2007</v>
       </c>
       <c r="L199" t="b">
         <v>1</v>
       </c>
       <c r="M199" t="n">
-        <v>4.17290189953575</v>
+        <v>88.135881202134</v>
       </c>
       <c r="N199" t="n">
-        <v>-0.151398517909744</v>
+        <v>-1.52267831398093</v>
       </c>
       <c r="O199" t="n">
-        <v>0.81958861886694</v>
+        <v>0.150234764324765</v>
       </c>
       <c r="P199" t="s">
         <v>23</v>
@@ -10263,34 +10263,34 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B200" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C200" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D200" t="s">
         <v>18</v>
       </c>
       <c r="E200" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="G200" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="H200" t="n">
-        <v>432</v>
+        <v>243</v>
       </c>
       <c r="I200" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J200" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="K200" t="n">
         <v>2023</v>
@@ -10299,13 +10299,13 @@
         <v>1</v>
       </c>
       <c r="M200" t="n">
-        <v>4.17288209344542</v>
+        <v>9.61203743135621</v>
       </c>
       <c r="N200" t="n">
-        <v>-0.151399197205583</v>
+        <v>0.083801251505233</v>
       </c>
       <c r="O200" t="n">
-        <v>0.819587742428702</v>
+        <v>0.831389753865606</v>
       </c>
       <c r="P200" t="s">
         <v>23</v>
@@ -10313,34 +10313,34 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B201" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C201" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D201" t="s">
         <v>18</v>
       </c>
       <c r="E201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F201" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="G201" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="H201" t="n">
-        <v>841</v>
+        <v>53</v>
       </c>
       <c r="I201" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J201" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="K201" t="n">
         <v>2023</v>
@@ -10349,13 +10349,13 @@
         <v>1</v>
       </c>
       <c r="M201" t="n">
-        <v>27.0389702137899</v>
+        <v>48.4483227965307</v>
       </c>
       <c r="N201" t="n">
-        <v>1.06249136556588</v>
+        <v>-0.491452101473701</v>
       </c>
       <c r="O201" t="n">
-        <v>0.131535963423934</v>
+        <v>0.503221346939231</v>
       </c>
       <c r="P201" t="s">
         <v>23</v>
@@ -10363,63 +10363,57 @@
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B202" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C202" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D202" t="s">
         <v>18</v>
       </c>
       <c r="E202" t="n">
+        <v>1</v>
+      </c>
+      <c r="F202" t="s">
+        <v>36</v>
+      </c>
+      <c r="G202" t="s">
+        <v>37</v>
+      </c>
+      <c r="H202" t="n">
+        <v>21</v>
+      </c>
+      <c r="I202" t="n">
         <v>2</v>
       </c>
-      <c r="F202" t="s">
-        <v>115</v>
-      </c>
-      <c r="G202" t="s">
-        <v>116</v>
-      </c>
-      <c r="H202" t="n">
-        <v>841</v>
-      </c>
-      <c r="I202" t="n">
-        <v>15</v>
-      </c>
       <c r="J202" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="K202" t="n">
         <v>2023</v>
       </c>
       <c r="L202" t="b">
-        <v>1</v>
-      </c>
-      <c r="M202" t="n">
-        <v>27.0389721308422</v>
-      </c>
-      <c r="N202" t="n">
-        <v>1.06249128763984</v>
-      </c>
-      <c r="O202" t="n">
-        <v>0.131535961470581</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M202"/>
+      <c r="N202"/>
+      <c r="O202"/>
       <c r="P202" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B203" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C203" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D203" t="s">
         <v>18</v>
@@ -10428,34 +10422,34 @@
         <v>1</v>
       </c>
       <c r="F203" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="G203" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="H203" t="n">
-        <v>413</v>
+        <v>90</v>
       </c>
       <c r="I203" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J203" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="K203" t="n">
-        <v>2007</v>
+        <v>2023</v>
       </c>
       <c r="L203" t="b">
         <v>1</v>
       </c>
       <c r="M203" t="n">
-        <v>88.1359321457827</v>
+        <v>54.1971893664919</v>
       </c>
       <c r="N203" t="n">
-        <v>-1.52268347944976</v>
+        <v>-0.898590661613937</v>
       </c>
       <c r="O203" t="n">
-        <v>0.150223160603143</v>
+        <v>0.256693517861474</v>
       </c>
       <c r="P203" t="s">
         <v>23</v>
@@ -10463,13 +10457,13 @@
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B204" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C204" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D204" t="s">
         <v>18</v>
@@ -10478,34 +10472,34 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="G204" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="H204" t="n">
-        <v>413</v>
+        <v>865</v>
       </c>
       <c r="I204" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J204" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="K204" t="n">
-        <v>2007</v>
+        <v>2023</v>
       </c>
       <c r="L204" t="b">
         <v>1</v>
       </c>
       <c r="M204" t="n">
-        <v>88.135881202134</v>
+        <v>62.3803683758874</v>
       </c>
       <c r="N204" t="n">
-        <v>-1.52267831398093</v>
+        <v>-0.142093117357641</v>
       </c>
       <c r="O204" t="n">
-        <v>0.150234764324765</v>
+        <v>0.687476157395656</v>
       </c>
       <c r="P204" t="s">
         <v>23</v>
@@ -10513,10 +10507,10 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B205" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C205" t="s">
         <v>17</v>
@@ -10528,34 +10522,34 @@
         <v>1</v>
       </c>
       <c r="F205" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G205" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H205" t="n">
-        <v>243</v>
+        <v>1200</v>
       </c>
       <c r="I205" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J205" t="n">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="K205" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="L205" t="b">
         <v>1</v>
       </c>
       <c r="M205" t="n">
-        <v>9.61203743135621</v>
+        <v>17.6000324086398</v>
       </c>
       <c r="N205" t="n">
-        <v>0.083801251505233</v>
+        <v>-0.177237750670174</v>
       </c>
       <c r="O205" t="n">
-        <v>0.831389753865606</v>
+        <v>0.214527791747208</v>
       </c>
       <c r="P205" t="s">
         <v>23</v>
@@ -10563,10 +10557,10 @@
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B206" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C206" t="s">
         <v>22</v>
@@ -10578,34 +10572,34 @@
         <v>1</v>
       </c>
       <c r="F206" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G206" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H206" t="n">
-        <v>53</v>
+        <v>1488</v>
       </c>
       <c r="I206" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J206" t="n">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="K206" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="L206" t="b">
         <v>1</v>
       </c>
       <c r="M206" t="n">
-        <v>48.4483227965307</v>
+        <v>24.3154629849416</v>
       </c>
       <c r="N206" t="n">
-        <v>-0.491452101473701</v>
+        <v>-0.107834394735686</v>
       </c>
       <c r="O206" t="n">
-        <v>0.503221346939231</v>
+        <v>0.554320609923393</v>
       </c>
       <c r="P206" t="s">
         <v>23</v>
@@ -10613,13 +10607,13 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B207" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C207" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D207" t="s">
         <v>18</v>
@@ -10628,42 +10622,48 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G207" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H207" t="n">
-        <v>21</v>
+        <v>468</v>
       </c>
       <c r="I207" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="J207" t="n">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="K207" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="L207" t="b">
-        <v>0</v>
-      </c>
-      <c r="M207"/>
-      <c r="N207"/>
-      <c r="O207"/>
+        <v>1</v>
+      </c>
+      <c r="M207" t="n">
+        <v>63.8845914773122</v>
+      </c>
+      <c r="N207" t="n">
+        <v>-1.756230414883</v>
+      </c>
+      <c r="O207" t="n">
+        <v>0.0916255144072397</v>
+      </c>
       <c r="P207" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B208" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C208" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D208" t="s">
         <v>18</v>
@@ -10672,48 +10672,42 @@
         <v>1</v>
       </c>
       <c r="F208" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G208" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H208" t="n">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="I208" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J208" t="n">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="K208" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L208" t="b">
         <v>1</v>
       </c>
-      <c r="M208" t="n">
-        <v>54.1971893664919</v>
-      </c>
-      <c r="N208" t="n">
-        <v>-0.898590661613937</v>
-      </c>
-      <c r="O208" t="n">
-        <v>0.256693517861474</v>
-      </c>
+      <c r="M208"/>
+      <c r="N208"/>
+      <c r="O208"/>
       <c r="P208" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B209" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C209" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D209" t="s">
         <v>18</v>
@@ -10722,34 +10716,34 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G209" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H209" t="n">
-        <v>865</v>
+        <v>142</v>
       </c>
       <c r="I209" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J209" t="n">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="K209" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="L209" t="b">
         <v>1</v>
       </c>
       <c r="M209" t="n">
-        <v>62.3803683758874</v>
+        <v>23.3866454027794</v>
       </c>
       <c r="N209" t="n">
-        <v>-0.142093117357641</v>
+        <v>-0.133993639774481</v>
       </c>
       <c r="O209" t="n">
-        <v>0.687476157395656</v>
+        <v>0.724482761673577</v>
       </c>
       <c r="P209" t="s">
         <v>23</v>
@@ -10763,7 +10757,7 @@
         <v>120</v>
       </c>
       <c r="C210" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D210" t="s">
         <v>18</v>
@@ -10778,7 +10772,7 @@
         <v>52</v>
       </c>
       <c r="H210" t="n">
-        <v>1200</v>
+        <v>722</v>
       </c>
       <c r="I210" t="n">
         <v>28</v>
@@ -10793,13 +10787,13 @@
         <v>1</v>
       </c>
       <c r="M210" t="n">
-        <v>17.6000324086398</v>
+        <v>17.2242004763788</v>
       </c>
       <c r="N210" t="n">
-        <v>-0.177237750670174</v>
+        <v>-0.0625775302178686</v>
       </c>
       <c r="O210" t="n">
-        <v>0.214527791747208</v>
+        <v>0.744513990778776</v>
       </c>
       <c r="P210" t="s">
         <v>23</v>
@@ -10813,7 +10807,7 @@
         <v>120</v>
       </c>
       <c r="C211" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D211" t="s">
         <v>18</v>
@@ -10828,7 +10822,7 @@
         <v>52</v>
       </c>
       <c r="H211" t="n">
-        <v>1488</v>
+        <v>3169</v>
       </c>
       <c r="I211" t="n">
         <v>28</v>
@@ -10843,13 +10837,13 @@
         <v>1</v>
       </c>
       <c r="M211" t="n">
-        <v>24.3154629849416</v>
+        <v>34.9836008250607</v>
       </c>
       <c r="N211" t="n">
-        <v>-0.107834394735686</v>
+        <v>-0.111791711877384</v>
       </c>
       <c r="O211" t="n">
-        <v>0.554320609923393</v>
+        <v>0.468476639281231</v>
       </c>
       <c r="P211" t="s">
         <v>23</v>
@@ -10857,13 +10851,13 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B212" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C212" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D212" t="s">
         <v>18</v>
@@ -10872,48 +10866,42 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G212" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H212" t="n">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="I212" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="J212" t="n">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="K212" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="L212" t="b">
-        <v>1</v>
-      </c>
-      <c r="M212" t="n">
-        <v>63.8845914773122</v>
-      </c>
-      <c r="N212" t="n">
-        <v>-1.756230414883</v>
-      </c>
-      <c r="O212" t="n">
-        <v>0.0916255144072397</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M212"/>
+      <c r="N212"/>
+      <c r="O212"/>
       <c r="P212" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B213" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C213" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D213" t="s">
         <v>18</v>
@@ -10922,42 +10910,48 @@
         <v>1</v>
       </c>
       <c r="F213" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G213" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H213" t="n">
-        <v>21</v>
+        <v>731</v>
       </c>
       <c r="I213" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="J213" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="K213" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="L213" t="b">
         <v>1</v>
       </c>
-      <c r="M213"/>
-      <c r="N213"/>
-      <c r="O213"/>
+      <c r="M213" t="n">
+        <v>25.3634545070029</v>
+      </c>
+      <c r="N213" t="n">
+        <v>0.888554138813603</v>
+      </c>
+      <c r="O213" t="n">
+        <v>0.0033753950342707</v>
+      </c>
       <c r="P213" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B214" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C214" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D214" t="s">
         <v>18</v>
@@ -10966,48 +10960,42 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G214" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H214" t="n">
-        <v>142</v>
+        <v>976</v>
       </c>
       <c r="I214" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J214" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="K214" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="L214" t="b">
         <v>1</v>
       </c>
-      <c r="M214" t="n">
-        <v>23.3866454027794</v>
-      </c>
-      <c r="N214" t="n">
-        <v>-0.133993639774481</v>
-      </c>
-      <c r="O214" t="n">
-        <v>0.724482761673577</v>
-      </c>
+      <c r="M214"/>
+      <c r="N214"/>
+      <c r="O214"/>
       <c r="P214" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B215" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C215" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D215" t="s">
         <v>18</v>
@@ -11016,48 +11004,42 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G215" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H215" t="n">
-        <v>722</v>
+        <v>2</v>
       </c>
       <c r="I215" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J215" t="n">
-        <v>1997</v>
+        <v>2016</v>
       </c>
       <c r="K215" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="L215" t="b">
-        <v>1</v>
-      </c>
-      <c r="M215" t="n">
-        <v>17.2242004763788</v>
-      </c>
-      <c r="N215" t="n">
-        <v>-0.0625775302178686</v>
-      </c>
-      <c r="O215" t="n">
-        <v>0.744513990778776</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M215"/>
+      <c r="N215"/>
+      <c r="O215"/>
       <c r="P215" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B216" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C216" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D216" t="s">
         <v>18</v>
@@ -11066,34 +11048,34 @@
         <v>1</v>
       </c>
       <c r="F216" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G216" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H216" t="n">
-        <v>3169</v>
+        <v>559</v>
       </c>
       <c r="I216" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J216" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="K216" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="L216" t="b">
         <v>1</v>
       </c>
       <c r="M216" t="n">
-        <v>34.9836008250607</v>
+        <v>36.5374750333899</v>
       </c>
       <c r="N216" t="n">
-        <v>-0.111791711877384</v>
+        <v>0.141924957308229</v>
       </c>
       <c r="O216" t="n">
-        <v>0.468476639281231</v>
+        <v>0.708114476390118</v>
       </c>
       <c r="P216" t="s">
         <v>23</v>
@@ -11107,7 +11089,7 @@
         <v>121</v>
       </c>
       <c r="C217" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D217" t="s">
         <v>18</v>
@@ -11122,25 +11104,31 @@
         <v>63</v>
       </c>
       <c r="H217" t="n">
-        <v>13</v>
+        <v>1684</v>
       </c>
       <c r="I217" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="J217" t="n">
-        <v>2018</v>
+        <v>1999</v>
       </c>
       <c r="K217" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="L217" t="b">
-        <v>0</v>
-      </c>
-      <c r="M217"/>
-      <c r="N217"/>
-      <c r="O217"/>
+        <v>1</v>
+      </c>
+      <c r="M217" t="n">
+        <v>33.7946272452919</v>
+      </c>
+      <c r="N217" t="n">
+        <v>0.282382323914653</v>
+      </c>
+      <c r="O217" t="n">
+        <v>0.391636122002955</v>
+      </c>
       <c r="P217" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="218">
@@ -11151,7 +11139,7 @@
         <v>121</v>
       </c>
       <c r="C218" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="D218" t="s">
         <v>18</v>
@@ -11166,262 +11154,24 @@
         <v>63</v>
       </c>
       <c r="H218" t="n">
-        <v>731</v>
+        <v>3</v>
       </c>
       <c r="I218" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="J218" t="n">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="K218" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L218" t="b">
-        <v>1</v>
-      </c>
-      <c r="M218" t="n">
-        <v>25.3634545070029</v>
-      </c>
-      <c r="N218" t="n">
-        <v>0.888554138813603</v>
-      </c>
-      <c r="O218" t="n">
-        <v>0.0033753950342707</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M218"/>
+      <c r="N218"/>
+      <c r="O218"/>
       <c r="P218" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>44</v>
-      </c>
-      <c r="B219" t="s">
-        <v>121</v>
-      </c>
-      <c r="C219" t="s">
-        <v>28</v>
-      </c>
-      <c r="D219" t="s">
-        <v>18</v>
-      </c>
-      <c r="E219" t="n">
-        <v>1</v>
-      </c>
-      <c r="F219" t="s">
-        <v>62</v>
-      </c>
-      <c r="G219" t="s">
-        <v>63</v>
-      </c>
-      <c r="H219" t="n">
-        <v>976</v>
-      </c>
-      <c r="I219" t="n">
-        <v>25</v>
-      </c>
-      <c r="J219" t="n">
-        <v>1999</v>
-      </c>
-      <c r="K219" t="n">
-        <v>2023</v>
-      </c>
-      <c r="L219" t="b">
-        <v>1</v>
-      </c>
-      <c r="M219"/>
-      <c r="N219"/>
-      <c r="O219"/>
-      <c r="P219" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>44</v>
-      </c>
-      <c r="B220" t="s">
-        <v>121</v>
-      </c>
-      <c r="C220" t="s">
-        <v>30</v>
-      </c>
-      <c r="D220" t="s">
-        <v>18</v>
-      </c>
-      <c r="E220" t="n">
-        <v>1</v>
-      </c>
-      <c r="F220" t="s">
-        <v>62</v>
-      </c>
-      <c r="G220" t="s">
-        <v>63</v>
-      </c>
-      <c r="H220" t="n">
-        <v>2</v>
-      </c>
-      <c r="I220" t="n">
-        <v>2</v>
-      </c>
-      <c r="J220" t="n">
-        <v>2016</v>
-      </c>
-      <c r="K220" t="n">
-        <v>2021</v>
-      </c>
-      <c r="L220" t="b">
-        <v>0</v>
-      </c>
-      <c r="M220"/>
-      <c r="N220"/>
-      <c r="O220"/>
-      <c r="P220" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>44</v>
-      </c>
-      <c r="B221" t="s">
-        <v>121</v>
-      </c>
-      <c r="C221" t="s">
-        <v>31</v>
-      </c>
-      <c r="D221" t="s">
-        <v>18</v>
-      </c>
-      <c r="E221" t="n">
-        <v>1</v>
-      </c>
-      <c r="F221" t="s">
-        <v>62</v>
-      </c>
-      <c r="G221" t="s">
-        <v>63</v>
-      </c>
-      <c r="H221" t="n">
-        <v>559</v>
-      </c>
-      <c r="I221" t="n">
-        <v>25</v>
-      </c>
-      <c r="J221" t="n">
-        <v>1999</v>
-      </c>
-      <c r="K221" t="n">
-        <v>2023</v>
-      </c>
-      <c r="L221" t="b">
-        <v>1</v>
-      </c>
-      <c r="M221" t="n">
-        <v>36.5374750333899</v>
-      </c>
-      <c r="N221" t="n">
-        <v>0.141924957308229</v>
-      </c>
-      <c r="O221" t="n">
-        <v>0.708114476390118</v>
-      </c>
-      <c r="P221" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>44</v>
-      </c>
-      <c r="B222" t="s">
-        <v>121</v>
-      </c>
-      <c r="C222" t="s">
-        <v>32</v>
-      </c>
-      <c r="D222" t="s">
-        <v>18</v>
-      </c>
-      <c r="E222" t="n">
-        <v>1</v>
-      </c>
-      <c r="F222" t="s">
-        <v>62</v>
-      </c>
-      <c r="G222" t="s">
-        <v>63</v>
-      </c>
-      <c r="H222" t="n">
-        <v>1684</v>
-      </c>
-      <c r="I222" t="n">
-        <v>25</v>
-      </c>
-      <c r="J222" t="n">
-        <v>1999</v>
-      </c>
-      <c r="K222" t="n">
-        <v>2023</v>
-      </c>
-      <c r="L222" t="b">
-        <v>1</v>
-      </c>
-      <c r="M222" t="n">
-        <v>33.7946272452919</v>
-      </c>
-      <c r="N222" t="n">
-        <v>0.282382323914653</v>
-      </c>
-      <c r="O222" t="n">
-        <v>0.391636122002955</v>
-      </c>
-      <c r="P222" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>44</v>
-      </c>
-      <c r="B223" t="s">
-        <v>121</v>
-      </c>
-      <c r="C223" t="s">
-        <v>66</v>
-      </c>
-      <c r="D223" t="s">
-        <v>18</v>
-      </c>
-      <c r="E223" t="n">
-        <v>1</v>
-      </c>
-      <c r="F223" t="s">
-        <v>62</v>
-      </c>
-      <c r="G223" t="s">
-        <v>63</v>
-      </c>
-      <c r="H223" t="n">
-        <v>3</v>
-      </c>
-      <c r="I223" t="n">
-        <v>3</v>
-      </c>
-      <c r="J223" t="n">
-        <v>2016</v>
-      </c>
-      <c r="K223" t="n">
-        <v>2021</v>
-      </c>
-      <c r="L223" t="b">
-        <v>0</v>
-      </c>
-      <c r="M223"/>
-      <c r="N223"/>
-      <c r="O223"/>
-      <c r="P223" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated figure names (St. Andrews Aquatic Preserve)
</commit_message>
<xml_diff>
--- a/SAV/output/website/SAV_BBpct_LMEresults_All.xlsx
+++ b/SAV/output/website/SAV_BBpct_LMEresults_All.xlsx
@@ -356,7 +356,7 @@
     <t xml:space="preserve">Rookery Bay National Estuarine Research Reserve</t>
   </si>
   <si>
-    <t xml:space="preserve">St. Andrews State Park Aquatic Preserve</t>
+    <t xml:space="preserve">St. Andrews Aquatic Preserve</t>
   </si>
   <si>
     <t xml:space="preserve">Central Panhandle Aquatic Preserves Seagrass Monitoring, St. Andrew Bay Aquatic Preserve Seagrass Monitoring</t>
@@ -10005,13 +10005,13 @@
         <v>1</v>
       </c>
       <c r="M194" t="n">
-        <v>84.4240875767503</v>
+        <v>84.4240525929707</v>
       </c>
       <c r="N194" t="n">
-        <v>-2.62425821800902</v>
+        <v>-2.62425693324902</v>
       </c>
       <c r="O194" t="n">
-        <v>0.0740365212949048</v>
+        <v>0.0740357901071176</v>
       </c>
       <c r="P194" t="s">
         <v>23</v>
@@ -10055,13 +10055,13 @@
         <v>1</v>
       </c>
       <c r="M195" t="n">
-        <v>11.9869803993408</v>
+        <v>11.9869804005955</v>
       </c>
       <c r="N195" t="n">
-        <v>0.27052871964274</v>
+        <v>0.270528719596189</v>
       </c>
       <c r="O195" t="n">
-        <v>0.485492239750769</v>
+        <v>0.485492239588718</v>
       </c>
       <c r="P195" t="s">
         <v>23</v>
@@ -10149,13 +10149,13 @@
         <v>1</v>
       </c>
       <c r="M197" t="n">
-        <v>4.17288209344542</v>
+        <v>4.17290189953575</v>
       </c>
       <c r="N197" t="n">
-        <v>-0.151399197205583</v>
+        <v>-0.151398517909744</v>
       </c>
       <c r="O197" t="n">
-        <v>0.819587742428702</v>
+        <v>0.81958861886694</v>
       </c>
       <c r="P197" t="s">
         <v>23</v>
@@ -10199,13 +10199,13 @@
         <v>1</v>
       </c>
       <c r="M198" t="n">
-        <v>27.0389702137899</v>
+        <v>27.0389721308422</v>
       </c>
       <c r="N198" t="n">
-        <v>1.06249136556588</v>
+        <v>1.06249128763984</v>
       </c>
       <c r="O198" t="n">
-        <v>0.131535963423934</v>
+        <v>0.131535961470581</v>
       </c>
       <c r="P198" t="s">
         <v>23</v>
@@ -10249,13 +10249,13 @@
         <v>1</v>
       </c>
       <c r="M199" t="n">
-        <v>88.135881202134</v>
+        <v>88.1359321457827</v>
       </c>
       <c r="N199" t="n">
-        <v>-1.52267831398093</v>
+        <v>-1.52268347944976</v>
       </c>
       <c r="O199" t="n">
-        <v>0.150234764324765</v>
+        <v>0.150223160603143</v>
       </c>
       <c r="P199" t="s">
         <v>23</v>

</xml_diff>